<commit_message>
delete comments and transfer print into ENG
</commit_message>
<xml_diff>
--- a/GRAMMAR/21_7.xlsx
+++ b/GRAMMAR/21_7.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,25 +440,30 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Fre</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>文法</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>含义</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>备注</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>rand</t>
         </is>
@@ -469,69 +474,82 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
         <v>3</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>〜どころか</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>别说…就连…</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>hello</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.7375353912353575</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
+        <v>27</v>
+      </c>
+      <c r="C3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>どうも〜らしい（ようだ、みたいだ）</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>推测</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>0.8270358291314149</v>
+          <t>申す</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>自谦敬语，自我介绍，道歉，请求</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>もうす</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0.6343311062272082</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>高度な</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>精确的</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
-        <v>0.3108714365923027</v>
+          <t>どうも〜らしい（ようだ、みたいだ）</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>推测</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>0.8270358291314149</v>
       </c>
     </row>
     <row r="5">
@@ -539,47 +557,57 @@
         <v>44</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>取り組み</t>
-        </is>
+        <v>19</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>举措；对策</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v>0.5384924006538645</v>
+          <t>にかけて</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>在…领域</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>～から～にかけて</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0.6996433895415878</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>無駄に</t>
-        </is>
+        <v>9</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>浪费</t>
+          <t>調子</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>むだに</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>0.03263709747300292</v>
+          <t>状况，样子</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ちょうし</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0.4359690322438915</v>
       </c>
     </row>
     <row r="7">
@@ -587,21 +615,24 @@
         <v>26</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>左右される</t>
-        </is>
+        <v>21</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>被影响</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>0.9197179488086107</v>
+          <t>にかかわらず</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>不论如何；不管怎样</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>0.6125091468653899</v>
       </c>
     </row>
     <row r="8">
@@ -609,25 +640,24 @@
         <v>27</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>申す</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>自谦敬语，自我介绍，道歉，请求</t>
+          <t>にあたって</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>もうす</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>0.6343311062272082</v>
+          <t>在……之际(重要时刻)</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>0.8508878993100624</v>
       </c>
     </row>
     <row r="9">
@@ -635,21 +665,24 @@
         <v>28</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>ずっと</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>…得多;很…</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>0.6081403016996318</v>
+          <t>のに</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>尽管;竟然;明明</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>0.9488407826814781</v>
       </c>
     </row>
     <row r="10">
@@ -657,21 +690,28 @@
         <v>29</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>〜ような</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>有种…样的感觉</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>0.796311995251986</v>
+          <t>N+すら</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>甚至～；连～</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>用于消极</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9549994854581604</v>
       </c>
     </row>
     <row r="11">
@@ -679,21 +719,24 @@
         <v>30</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>〜ことに</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>令人感到…的是…</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="n">
-        <v>0.9879720579766592</v>
+          <t>にかぎって</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>偏偏…；只…</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>0.07299646371122037</v>
       </c>
     </row>
     <row r="12">
@@ -701,21 +744,28 @@
         <v>31</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>うえに</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>不仅…而且…</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="n">
-        <v>0.5126565689286083</v>
+          <t>さえ</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>极端的例子，从而类推其它事物</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>中性词</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1330594331586105</v>
       </c>
     </row>
     <row r="13">
@@ -723,25 +773,24 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>くせに</t>
-        </is>
+        <v>7</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>明明；却</t>
+          <t>ほど</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>主语一致</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>0.6234540758851841</v>
+          <t>程度</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>0.9963776270812551</v>
       </c>
     </row>
     <row r="14">
@@ -749,91 +798,107 @@
         <v>33</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ていない</t>
-        </is>
+        <v>8</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>现在处于未发生的状态</t>
+          <t>A は B ほど C ない</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>后面不能直接{と}，而是{しないと}</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>0.6927616718677013</v>
+          <t>A没有B那么……</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>0.8235889125904149</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>少なくとも</t>
-        </is>
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>至少；起码</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
-        <v>0.5483486299794592</v>
+          <t>おかしい</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>奇怪的；滑稽的</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>0.06795000018538722</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>だるい</t>
-        </is>
+        <v>18</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>疲倦的；无力的</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>0.1491314804966607</v>
+          <t>を問わず</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>不论，不管</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>をとわず</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0.1806502985817318</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>やりだす</t>
-        </is>
+        <v>22</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>开始做；着手进行</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
-        <v>0.7069130217446928</v>
+          <t>めった</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>几乎不…</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>后接否定</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>0.8988080151797992</v>
       </c>
     </row>
     <row r="18">
@@ -841,21 +906,28 @@
         <v>37</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>申し上げる</t>
-        </is>
+        <v>12</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>「言う」的自谦语</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="n">
-        <v>0.7106186444294472</v>
+          <t>なら</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>既然你提到…的话</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>对方说的话被当成一个讨论的主题</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>0.5345819677170777</v>
       </c>
     </row>
     <row r="19">
@@ -863,21 +935,28 @@
         <v>38</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>に際して</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>当...之际(契机)</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="n">
-        <v>0.2315365082224048</v>
+          <t>ちっとも</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>一点也不…</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>后接否定</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>0.9726306105491628</v>
       </c>
     </row>
     <row r="20">
@@ -885,25 +964,24 @@
         <v>39</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>伺う</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>「聞く·尋ねる·問う」的自谦</t>
+          <t>において</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>うかがう</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>0.4611913730264156</v>
+          <t>在…方面；在…时候；在…地点</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>0.9534891008814962</v>
       </c>
     </row>
     <row r="21">
@@ -911,21 +989,24 @@
         <v>40</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>ちゃって</t>
-        </is>
+        <v>15</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>てしまう口语</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="n">
-        <v>0.5054651805992773</v>
+          <t>まさか</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>(1)难道… (2)该不会…吧 (3)怎么可能</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="n">
+        <v>0.3920945581172406</v>
       </c>
     </row>
     <row r="22">
@@ -933,87 +1014,103 @@
         <v>41</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>だし</t>
-        </is>
+        <v>16</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>因果，理由</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="n">
-        <v>0.8713752555540851</v>
+          <t>どなた</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>哪位人</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>0.8221365827612416</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>〜の一つ</t>
-        </is>
+        <v>20</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>〜之一</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
-        <v>0.2711777193583428</v>
+          <t>にもかかわらず</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>虽然</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>0.5050196341474035</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>取り入れる</t>
-        </is>
+        <v>17</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>引进;采纳</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="n">
-        <v>0.4783192196107933</v>
+          <t>を通して</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>(1)通过…(人，媒介，经验)(2)在…期间</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>0.7505104828225797</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>言われた</t>
-        </is>
+        <v>11</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>有人曾说;被说</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="n">
-        <v>0.1975445518462655</v>
+          <t>だったら</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>如果…的话</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>对方说的话被当成一个既定事实</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>0.08635883665735966</v>
       </c>
     </row>
     <row r="26">
@@ -1021,69 +1118,74 @@
         <v>23</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>どうも</t>
-        </is>
+        <v>35</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>(1)似乎；总觉得 (2)十分；非常；实在</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="n">
-        <v>0.09752777340865859</v>
+          <t>言われた</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>有人曾说;被说</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="n">
+        <v>0.1975445518462655</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>めった</t>
-        </is>
+        <v>23</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>几乎不…</t>
+          <t>どうも</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>后接否定</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>0.8988080151797992</v>
+          <t>(1)似乎；总觉得 (2)十分；非常；实在</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="n">
+        <v>0.09752777340865859</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>にかかわらず</t>
-        </is>
+        <v>43</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>不论如何；不管怎样</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="n">
-        <v>0.6125091468653899</v>
+          <t>取り入れる</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>引进;采纳</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="n">
+        <v>0.4783192196107933</v>
       </c>
     </row>
     <row r="29">
@@ -1091,21 +1193,24 @@
         <v>2</v>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>にあたって</t>
-        </is>
+        <v>45</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>在……之际(重要时刻)</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="n">
-        <v>0.8508878993100624</v>
+          <t>高度な</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>精确的</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="n">
+        <v>0.3108714365923027</v>
       </c>
     </row>
     <row r="30">
@@ -1113,21 +1218,24 @@
         <v>3</v>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>のに</t>
-        </is>
+        <v>44</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>尽管;竟然;明明</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="n">
-        <v>0.9488407826814781</v>
+          <t>取り組み</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>举措；对策</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="n">
+        <v>0.5384924006538645</v>
       </c>
     </row>
     <row r="31">
@@ -1135,25 +1243,28 @@
         <v>4</v>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>N+すら</t>
-        </is>
+        <v>25</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>甚至～；连～</t>
+          <t>無駄に</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>用于消极</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
-        <v>0.9549994854581604</v>
+          <t>浪费</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>むだに</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>0.03263709747300292</v>
       </c>
     </row>
     <row r="32">
@@ -1161,379 +1272,411 @@
         <v>5</v>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>にかぎって</t>
-        </is>
+        <v>26</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>偏偏…；只…</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="n">
-        <v>0.07299646371122037</v>
+          <t>左右される</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>被影响</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="n">
+        <v>0.9197179488086107</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>さえ</t>
-        </is>
+        <v>28</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>极端的例子，从而类推其它事物</t>
+          <t>ずっと</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>中性词</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
-        <v>0.1330594331586105</v>
+          <t>…得多;很…</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="n">
+        <v>0.6081403016996318</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>ほど</t>
-        </is>
+        <v>29</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>程度</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="n">
-        <v>0.9963776270812551</v>
+          <t>〜ような</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>有种…样的感觉</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="n">
+        <v>0.796311995251986</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>A は B ほど C ない</t>
-        </is>
+        <v>30</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>A没有B那么……</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="n">
-        <v>0.8235889125904149</v>
+          <t>〜ことに</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>令人感到…的是…</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="n">
+        <v>0.9879720579766592</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>調子</t>
-        </is>
+        <v>31</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>状况，样子</t>
+          <t>うえに</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>ちょうし</t>
-        </is>
-      </c>
-      <c r="F36" t="n">
-        <v>0.4359690322438915</v>
+          <t>不仅…而且…</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="n">
+        <v>0.5126565689286083</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>おかしい</t>
-        </is>
+        <v>32</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>奇怪的；滑稽的</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="n">
-        <v>0.06795000018538722</v>
+          <t>くせに</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>明明；却</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>主语一致</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>0.6234540758851841</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>だったら</t>
-        </is>
+        <v>33</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>如果…的话</t>
+          <t>ていない</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>对方说的话被当成一个既定事实</t>
-        </is>
-      </c>
-      <c r="F38" t="n">
-        <v>0.08635883665735966</v>
+          <t>现在处于未发生的状态</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>后面不能直接{と}，而是{しないと}</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>0.6927616718677013</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B39" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>なら</t>
-        </is>
+        <v>34</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>既然你提到…的话</t>
+          <t>少なくとも</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>对方说的话被当成一个讨论的主题</t>
-        </is>
-      </c>
-      <c r="F39" t="n">
-        <v>0.5345819677170777</v>
+          <t>至少；起码</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="n">
+        <v>0.5483486299794592</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>ちっとも</t>
-        </is>
+        <v>24</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>一点也不…</t>
+          <t>だるい</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>后接否定</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
-        <v>0.9726306105491628</v>
+          <t>疲倦的；无力的</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="n">
+        <v>0.1491314804966607</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>において</t>
-        </is>
+        <v>36</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>在…方面；在…时候；在…地点</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="n">
-        <v>0.9534891008814962</v>
+          <t>やりだす</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>开始做；着手进行</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="n">
+        <v>0.7069130217446928</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>まさか</t>
-        </is>
+        <v>37</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>(1)难道… (2)该不会…吧 (3)怎么可能</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="n">
-        <v>0.3920945581172406</v>
+          <t>申し上げる</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>「言う」的自谦语</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="n">
+        <v>0.7106186444294472</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B43" t="n">
-        <v>0</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>どなた</t>
-        </is>
+        <v>38</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>哪位人</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="n">
-        <v>0.8221365827612416</v>
+          <t>に際して</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>当...之际(契机)</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="n">
+        <v>0.2315365082224048</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>を通して</t>
-        </is>
+        <v>39</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>(1)通过…(人，媒介，经验)(2)在…期间</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="n">
-        <v>0.7505104828225797</v>
+          <t>伺う</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>「聞く·尋ねる·問う」的自谦</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>うかがう</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>0.4611913730264156</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B45" t="n">
-        <v>0</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>を問わず</t>
-        </is>
+        <v>40</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>不论，不管</t>
+          <t>ちゃって</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>をとわず</t>
-        </is>
-      </c>
-      <c r="F45" t="n">
-        <v>0.1806502985817318</v>
+          <t>てしまう口语</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="n">
+        <v>0.5054651805992773</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>にかけて</t>
-        </is>
+        <v>41</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>在…领域</t>
+          <t>だし</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>～から～にかけて</t>
-        </is>
-      </c>
-      <c r="F46" t="n">
-        <v>0.6996433895415878</v>
+          <t>因果，理由</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="n">
+        <v>0.8713752555540851</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>にもかかわらず</t>
-        </is>
+        <v>42</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>虽然</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="n">
-        <v>0.5050196341474035</v>
+          <t>〜の一つ</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>〜之一</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="n">
+        <v>0.2711777193583428</v>
       </c>
     </row>
     <row r="48">
@@ -1541,20 +1684,23 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C48" t="inlineStr">
+        <v>46</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="inlineStr">
         <is>
           <t>売り上げ</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>销售额；营业额</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr"/>
-      <c r="F48" t="n">
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="n">
         <v>0.9112402273331391</v>
       </c>
     </row>

</xml_diff>